<commit_message>
Small changes on XLSForms
</commit_message>
<xml_diff>
--- a/xforms/testodk.xlsx
+++ b/xforms/testodk.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76">
   <si>
     <t>type</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Write something about the Household</t>
+  </si>
+  <si>
+    <t>note</t>
   </si>
   <si>
     <t>resultTest</t>
@@ -1316,7 +1319,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8768115942029" defaultRowHeight="11.75"/>
@@ -1499,41 +1502,41 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="9" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G9" s="10"/>
       <c r="I9" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K11" s="9" t="b">
         <v>1</v>
@@ -1768,172 +1771,172 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" ht="14.5" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="14.5" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="7">
         <v>2</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" ht="14.5" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7">
         <v>3</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" ht="14.5" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="7">
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" ht="14.5" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="7">
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" ht="14.5" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7" s="7">
         <v>6</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" ht="14.5" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="7">
         <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" ht="14.5" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="7">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" ht="14.5" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="7">
         <v>9</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" ht="14.5" spans="1:5">
@@ -2359,27 +2362,27 @@
   <sheetData>
     <row r="1" ht="14.55" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" ht="14.55" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>